<commit_message>
Updated README, TROUBLESHOOTING, & lessons learned
</commit_message>
<xml_diff>
--- a/docs/Project_Tracker.xlsx
+++ b/docs/Project_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://potbelly-my.sharepoint.com/personal/anicia_clayton_potbelly_com/Documents/Desktop/linguallearn-portfolio/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_1B14DB0FC593A75196C6933F0CB991BF92D0DE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DCC48FF-FC5D-430B-9EBE-23E0F6BE1FAB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{CE5F785D-15DF-442D-BF02-6C94E5833220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="389">
   <si>
     <t>LINGUALLEARN AI - PROJECT TRACKER</t>
   </si>
@@ -1192,12 +1192,21 @@
   <si>
     <t>Demonstrates ability to deliver projects</t>
   </si>
+  <si>
+    <t>Remove nested repo</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Git sync issue</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1249,8 +1258,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1299,6 +1313,18 @@
         <bgColor rgb="FFC00000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1327,7 +1353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1358,9 +1384,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1379,12 +1402,27 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFEB9C"/>
+      <color rgb="FFC6EFCE"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1684,7 +1722,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1699,100 +1737,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -1801,27 +1839,27 @@
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
     </row>
     <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -2099,24 +2137,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>342</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>343</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -2151,14 +2189,14 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>352</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -2193,14 +2231,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -2235,14 +2273,14 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="18" t="s">
         <v>370</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -2269,14 +2307,14 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="18" t="s">
         <v>377</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -2329,7 +2367,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2346,18 +2384,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -2409,8 +2447,8 @@
       <c r="C5" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>79</v>
+      <c r="D5" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>25</v>
@@ -2437,8 +2475,8 @@
       <c r="C6" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>79</v>
+      <c r="D6" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>25</v>
@@ -2465,8 +2503,8 @@
       <c r="C7" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>79</v>
+      <c r="D7" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>25</v>
@@ -2493,8 +2531,8 @@
       <c r="C8" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>79</v>
+      <c r="D8" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>25</v>
@@ -2521,8 +2559,8 @@
       <c r="C9" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>79</v>
+      <c r="D9" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>25</v>
@@ -2551,8 +2589,8 @@
       <c r="C10" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>79</v>
+      <c r="D10" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>25</v>
@@ -2579,8 +2617,8 @@
       <c r="C11" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>79</v>
+      <c r="D11" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>25</v>
@@ -2607,8 +2645,8 @@
       <c r="C12" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>79</v>
+      <c r="D12" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>25</v>
@@ -2637,8 +2675,8 @@
       <c r="C13" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>79</v>
+      <c r="D13" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>25</v>
@@ -2665,8 +2703,8 @@
       <c r="C14" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>79</v>
+      <c r="D14" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>25</v>
@@ -2693,8 +2731,8 @@
       <c r="C15" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>79</v>
+      <c r="D15" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>25</v>
@@ -2721,8 +2759,8 @@
       <c r="C16" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>79</v>
+      <c r="D16" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>25</v>
@@ -2749,8 +2787,8 @@
       <c r="C17" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>79</v>
+      <c r="D17" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>25</v>
@@ -2777,8 +2815,8 @@
       <c r="C18" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>79</v>
+      <c r="D18" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>25</v>
@@ -2817,7 +2855,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2834,18 +2872,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -2897,8 +2935,8 @@
       <c r="C5" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>79</v>
+      <c r="D5" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>25</v>
@@ -2925,8 +2963,8 @@
       <c r="C6" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>79</v>
+      <c r="D6" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>25</v>
@@ -2953,8 +2991,8 @@
       <c r="C7" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>79</v>
+      <c r="D7" s="23" t="s">
+        <v>387</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>25</v>
@@ -2981,10 +3019,10 @@
       <c r="C8" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="14" t="s">
+      <c r="D8" s="23" t="s">
+        <v>387</v>
+      </c>
+      <c r="E8" s="22" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -3016,7 +3054,7 @@
       <c r="D9" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="24" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="12" t="s">
@@ -3028,8 +3066,12 @@
       <c r="H9" s="11">
         <v>0</v>
       </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
+      <c r="I9" s="23" t="s">
+        <v>388</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
@@ -3518,24 +3560,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4170,24 +4212,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4822,24 +4864,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>37</v>
       </c>
     </row>
@@ -5446,24 +5488,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>37</v>
       </c>
     </row>
@@ -6095,17 +6137,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>322</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -6137,31 +6179,31 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="16" t="s">
+      <c r="E4" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="H4" s="16" t="s">
+      <c r="G4" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="I4" s="16"/>
+      <c r="I4" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6188,14 +6230,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>331</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">

</xml_diff>

<commit_message>
Updated README & Tracker
</commit_message>
<xml_diff>
--- a/docs/Project_Tracker.xlsx
+++ b/docs/Project_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://potbelly-my.sharepoint.com/personal/anicia_clayton_potbelly_com/Documents/Desktop/linguallearn-portfolio/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9127442-2913-40DC-8B94-276E6D9B79DE}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D277315-3308-49CD-B492-07CD0111A158}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1207,13 +1207,13 @@
     <t>AI Engineer Portfolio</t>
   </si>
   <si>
-    <t>26 (20%)</t>
-  </si>
-  <si>
-    <t>106 (80%)</t>
-  </si>
-  <si>
-    <t>27.5 / 90</t>
+    <t>30 / 90</t>
+  </si>
+  <si>
+    <t>30 (26%)</t>
+  </si>
+  <si>
+    <t>102 (77%)</t>
   </si>
 </sst>
 </file>
@@ -1698,6 +1698,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1986,7 +1990,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2197,7 +2201,7 @@
       </c>
       <c r="F16" s="18">
         <f>IFERROR(COUNTIF('Phase 2 - API &amp; Compute'!E5:E100,"Complete")/COUNTA('Phase 2 - API &amp; Compute'!A5:A100),0)</f>
-        <v>0.5714285714285714</v>
+        <v>0.76190476190476186</v>
       </c>
       <c r="G16" s="4">
         <f>COUNTIF('Phase 2 - API &amp; Compute'!E:E,"Blocked")</f>
@@ -2330,7 +2334,7 @@
         <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2354,7 +2358,7 @@
         <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -2373,7 +2377,7 @@
         <v>55</v>
       </c>
       <c r="B31" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -3148,7 +3152,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3576,7 +3580,7 @@
         <v>70</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>71</v>
@@ -3585,7 +3589,7 @@
         <v>1.5</v>
       </c>
       <c r="H17" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
@@ -3604,7 +3608,7 @@
         <v>70</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>71</v>
@@ -3613,7 +3617,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="11">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
@@ -3632,7 +3636,7 @@
         <v>70</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>71</v>
@@ -3641,7 +3645,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="11">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
@@ -3660,7 +3664,7 @@
         <v>70</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>98</v>
@@ -3669,7 +3673,7 @@
         <v>0.5</v>
       </c>
       <c r="H20" s="11">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
@@ -3688,7 +3692,7 @@
         <v>70</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Add S3 buckets and CloudFront for video delivery
</commit_message>
<xml_diff>
--- a/docs/Project_Tracker.xlsx
+++ b/docs/Project_Tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://potbelly-my.sharepoint.com/personal/anicia_clayton_potbelly_com/Documents/Desktop/linguallearn-portfolio/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAE68A4D-9389-4AFB-93A9-FD2E9A7D67D0}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA72ED7A-F606-4C9B-90A7-8B817274B6C2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1198,15 +1198,6 @@
     <t>In progress</t>
   </si>
   <si>
-    <t>40 / 120</t>
-  </si>
-  <si>
-    <t>35 (27%)</t>
-  </si>
-  <si>
-    <t>97 (73%)</t>
-  </si>
-  <si>
     <t>Phase 3 - Multi-Modal Layer</t>
   </si>
   <si>
@@ -1217,6 +1208,15 @@
   </si>
   <si>
     <t>7 Weeks (90-120 hours total)</t>
+  </si>
+  <si>
+    <t>45 / 120</t>
+  </si>
+  <si>
+    <t>39 (30%)</t>
+  </si>
+  <si>
+    <t>93 (70%)</t>
   </si>
 </sst>
 </file>
@@ -1471,6 +1471,11 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1482,11 +1487,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1995,8 +1995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2011,100 +2011,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="A1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="30" t="s">
         <v>380</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="27" t="s">
-        <v>388</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="B5" s="30" t="s">
+        <v>385</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="27" t="s">
-        <v>385</v>
-      </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="B7" s="30" t="s">
+        <v>382</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="27" t="s">
-        <v>386</v>
-      </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+      <c r="B8" s="30" t="s">
+        <v>383</v>
+      </c>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -2113,27 +2113,27 @@
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>387</v>
-      </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="B10" s="30" t="s">
+        <v>384</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
     </row>
     <row r="13" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
     </row>
     <row r="14" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -2196,7 +2196,7 @@
       <c r="B16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="27" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -2235,7 +2235,7 @@
       </c>
       <c r="F17" s="16">
         <f>IFERROR(COUNTIF('Phase 3 - Multi-Modal'!E5:E100,"Complete")/COUNTA('Phase 3 - Multi-Modal'!A5:A100),0)</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G17" s="4">
         <f>COUNTIF('Phase 3 - Multi-Modal'!E:E,"Blocked")</f>
@@ -2340,7 +2340,7 @@
         <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2364,7 +2364,7 @@
         <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -2383,7 +2383,7 @@
         <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -2426,24 +2426,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>331</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="4" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="29" t="s">
         <v>332</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -2478,14 +2478,14 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="29" t="s">
         <v>341</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -2520,14 +2520,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="29" t="s">
         <v>350</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -2562,14 +2562,14 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="29" t="s">
         <v>359</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -2596,14 +2596,14 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="29" t="s">
         <v>366</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -2673,18 +2673,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -3175,24 +3175,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="26" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3860,7 +3860,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3877,24 +3877,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="28" t="s">
         <v>381</v>
       </c>
     </row>
@@ -3944,7 +3944,7 @@
         <v>66</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>67</v>
@@ -3953,7 +3953,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
@@ -3972,7 +3972,7 @@
         <v>66</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>67</v>
@@ -3981,7 +3981,7 @@
         <v>0.5</v>
       </c>
       <c r="H6" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
@@ -4000,7 +4000,7 @@
         <v>66</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>67</v>
@@ -4028,7 +4028,7 @@
         <v>66</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>67</v>
@@ -4037,7 +4037,7 @@
         <v>1.5</v>
       </c>
       <c r="H8" s="10">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -4056,7 +4056,7 @@
         <v>66</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>94</v>
@@ -4065,7 +4065,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -4084,7 +4084,7 @@
         <v>66</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>67</v>
@@ -4543,18 +4543,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -5209,18 +5209,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -5847,18 +5847,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -6512,17 +6512,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>311</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -6639,14 +6639,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>324</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">

</xml_diff>

<commit_message>
Add Lambda function for video processing
</commit_message>
<xml_diff>
--- a/docs/Project_Tracker.xlsx
+++ b/docs/Project_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://potbelly-my.sharepoint.com/personal/anicia_clayton_potbelly_com/Documents/Desktop/linguallearn-portfolio/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA72ED7A-F606-4C9B-90A7-8B817274B6C2}"/>
+  <xr:revisionPtr revIDLastSave="231" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EC2CE71-16DC-497E-97AA-FF46821CF4EA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="400">
   <si>
     <t>LINGUALLEARN AI - PROJECT TRACKER</t>
   </si>
@@ -1210,13 +1210,46 @@
     <t>7 Weeks (90-120 hours total)</t>
   </si>
   <si>
-    <t>45 / 120</t>
-  </si>
-  <si>
-    <t>39 (30%)</t>
-  </si>
-  <si>
-    <t>93 (70%)</t>
+    <t>Later enhancement</t>
+  </si>
+  <si>
+    <t>Create Lambda Handler for Video Metadata</t>
+  </si>
+  <si>
+    <t>Create Lambda Infrastructure in Terraform</t>
+  </si>
+  <si>
+    <t>Package and Deploy Lambda Function</t>
+  </si>
+  <si>
+    <t>Test Lambda with S3 Upload</t>
+  </si>
+  <si>
+    <t>Verify S3 Event Triggers</t>
+  </si>
+  <si>
+    <t>P3-T021</t>
+  </si>
+  <si>
+    <t>P3-T022</t>
+  </si>
+  <si>
+    <t>P3-T023</t>
+  </si>
+  <si>
+    <t>P3-T024</t>
+  </si>
+  <si>
+    <t>P3-T025</t>
+  </si>
+  <si>
+    <t>54.5 / 120</t>
+  </si>
+  <si>
+    <t>49 (36%)</t>
+  </si>
+  <si>
+    <t>84 (61%)</t>
   </si>
 </sst>
 </file>
@@ -1996,7 +2029,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2234,8 +2267,8 @@
         <v>31</v>
       </c>
       <c r="F17" s="16">
-        <f>IFERROR(COUNTIF('Phase 3 - Multi-Modal'!E5:E100,"Complete")/COUNTA('Phase 3 - Multi-Modal'!A5:A100),0)</f>
-        <v>0.2</v>
+        <f>IFERROR(COUNTIF('Phase 3 - Multi-Modal'!E5:E105,"Complete")/COUNTA('Phase 3 - Multi-Modal'!A5:A105),0)</f>
+        <v>0.52</v>
       </c>
       <c r="G17" s="4">
         <f>COUNTIF('Phase 3 - Multi-Modal'!E:E,"Blocked")</f>
@@ -2332,7 +2365,7 @@
       </c>
       <c r="B24">
         <f>COUNTA('Phase 1 - Infrastructure'!A:A)+COUNTA('Phase 2 - API &amp; Compute'!A:A)+COUNTA('Phase 3 - Multi-Modal'!A:A)+COUNTA('Phase 4 - ML Integration'!A:A)+COUNTA('Phase 5 - Monitoring'!A:A)+COUNTA('Phase 6 - CICD'!A:A)</f>
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -2340,7 +2373,7 @@
         <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>387</v>
+        <v>398</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2364,7 +2397,7 @@
         <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>388</v>
+        <v>399</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -2383,7 +2416,7 @@
         <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>386</v>
+        <v>397</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -3856,11 +3889,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4000,7 +4033,7 @@
         <v>66</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>67</v>
@@ -4009,7 +4042,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
@@ -4084,7 +4117,7 @@
         <v>66</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>67</v>
@@ -4093,7 +4126,7 @@
         <v>2</v>
       </c>
       <c r="H10" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
@@ -4124,7 +4157,9 @@
         <v>0</v>
       </c>
       <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
+      <c r="J11" s="10" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
@@ -4140,7 +4175,7 @@
         <v>66</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>67</v>
@@ -4149,7 +4184,7 @@
         <v>0.5</v>
       </c>
       <c r="H12" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
@@ -4168,7 +4203,7 @@
         <v>66</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>67</v>
@@ -4177,7 +4212,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
@@ -4190,13 +4225,13 @@
         <v>83</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>169</v>
+        <v>387</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>67</v>
@@ -4205,7 +4240,7 @@
         <v>2</v>
       </c>
       <c r="H14" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
@@ -4218,22 +4253,22 @@
         <v>83</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>171</v>
+        <v>388</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>67</v>
       </c>
       <c r="G15" s="10">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H15" s="10">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
@@ -4246,13 +4281,13 @@
         <v>83</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>173</v>
+        <v>389</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>67</v>
@@ -4261,7 +4296,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
@@ -4271,25 +4306,25 @@
         <v>174</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>175</v>
+        <v>390</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>67</v>
       </c>
       <c r="G17" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H17" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
@@ -4299,25 +4334,25 @@
         <v>176</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>177</v>
+        <v>391</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="11" t="s">
         <v>94</v>
       </c>
       <c r="G18" s="10">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H18" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
@@ -4327,10 +4362,10 @@
         <v>178</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>66</v>
@@ -4338,11 +4373,11 @@
       <c r="E19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>94</v>
+      <c r="F19" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="G19" s="10">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H19" s="10">
         <v>0</v>
@@ -4355,10 +4390,10 @@
         <v>180</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>66</v>
@@ -4366,8 +4401,8 @@
       <c r="E20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>94</v>
+      <c r="F20" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="G20" s="10">
         <v>1</v>
@@ -4383,10 +4418,10 @@
         <v>182</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>66</v>
@@ -4394,11 +4429,11 @@
       <c r="E21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>94</v>
+      <c r="F21" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="G21" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H21" s="10">
         <v>0</v>
@@ -4411,10 +4446,10 @@
         <v>184</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>66</v>
@@ -4426,7 +4461,7 @@
         <v>67</v>
       </c>
       <c r="G22" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" s="10">
         <v>0</v>
@@ -4439,10 +4474,10 @@
         <v>186</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>66</v>
@@ -4450,11 +4485,11 @@
       <c r="E23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="11" t="s">
-        <v>67</v>
+      <c r="F23" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="G23" s="10">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H23" s="10">
         <v>0</v>
@@ -4467,10 +4502,10 @@
         <v>188</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>66</v>
@@ -4479,22 +4514,162 @@
         <v>29</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="G24" s="10">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="H24" s="10">
         <v>0</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G25" s="10">
+        <v>1</v>
+      </c>
+      <c r="H25" s="10">
+        <v>0</v>
+      </c>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="H26" s="10">
+        <v>0</v>
+      </c>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="10">
+        <v>1</v>
+      </c>
+      <c r="H27" s="10">
+        <v>0</v>
+      </c>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0</v>
+      </c>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G29" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="H29" s="10">
+        <v>0</v>
+      </c>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E5:E100">
+  <conditionalFormatting sqref="E5:E105">
     <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
@@ -4509,10 +4684,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" errorTitle="Invalid Entry" error="Invalid status" sqref="E5 E6 E7 E8 E9 E10 E11 E12 E13 E14 E15 E16 E17 E18 E19 E20 E21 E22 E23 E24 E25" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" errorTitle="Invalid Entry" error="Invalid status" sqref="E5 E6 E7 E8 E9 E10 E11 E12 E13:E18 E19 E20 E21 E22 E23 E24 E25 E26 E27 E28 E29 E30" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Not Started,In Progress,Complete,Blocked"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorTitle="Invalid Entry" error="Invalid priority" sqref="F5 F6 F7 F8 F9 F10 F11 F12 F13 F14 F15 F16 F17 F18 F19 F20 F21 F22 F23 F24 F25" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" errorTitle="Invalid Entry" error="Invalid priority" sqref="F5 F6 F7 F8 F9 F10 F11 F12 F13:F18 F19 F20 F21 F22 F23 F24 F25 F26 F27 F28 F29 F30" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add ASL vocabulary API endpoints
</commit_message>
<xml_diff>
--- a/docs/Project_Tracker.xlsx
+++ b/docs/Project_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://potbelly-my.sharepoint.com/personal/anicia_clayton_potbelly_com/Documents/Desktop/linguallearn-portfolio/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="231" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EC2CE71-16DC-497E-97AA-FF46821CF4EA}"/>
+  <xr:revisionPtr revIDLastSave="246" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F93A003E-78FC-4C25-9955-E34EDEC749E5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="📊 Project Overview" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="402">
   <si>
     <t>LINGUALLEARN AI - PROJECT TRACKER</t>
   </si>
@@ -1243,13 +1243,19 @@
     <t>P3-T025</t>
   </si>
   <si>
-    <t>54.5 / 120</t>
-  </si>
-  <si>
-    <t>49 (36%)</t>
-  </si>
-  <si>
-    <t>84 (61%)</t>
+    <t>Authentication error</t>
+  </si>
+  <si>
+    <t>Reset Secret</t>
+  </si>
+  <si>
+    <t>58 / 120</t>
+  </si>
+  <si>
+    <t>51 (37%)</t>
+  </si>
+  <si>
+    <t>82 (60%)</t>
   </si>
 </sst>
 </file>
@@ -2028,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2268,7 +2274,7 @@
       </c>
       <c r="F17" s="16">
         <f>IFERROR(COUNTIF('Phase 3 - Multi-Modal'!E5:E105,"Complete")/COUNTA('Phase 3 - Multi-Modal'!A5:A105),0)</f>
-        <v>0.52</v>
+        <v>0.6</v>
       </c>
       <c r="G17" s="4">
         <f>COUNTIF('Phase 3 - Multi-Modal'!E:E,"Blocked")</f>
@@ -2373,7 +2379,7 @@
         <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2397,7 +2403,7 @@
         <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -2416,7 +2422,7 @@
         <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -3891,9 +3897,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4371,7 +4377,7 @@
         <v>66</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>67</v>
@@ -4380,10 +4386,14 @@
         <v>2</v>
       </c>
       <c r="H19" s="10">
-        <v>0</v>
-      </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
+        <v>2.5</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
@@ -4399,7 +4409,7 @@
         <v>66</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>67</v>
@@ -4408,7 +4418,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>

</xml_diff>

<commit_message>
Added Phase 3 test suite & updated documentation
</commit_message>
<xml_diff>
--- a/docs/Project_Tracker.xlsx
+++ b/docs/Project_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://potbelly-my.sharepoint.com/personal/anicia_clayton_potbelly_com/Documents/Desktop/linguallearn-portfolio/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="246" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F93A003E-78FC-4C25-9955-E34EDEC749E5}"/>
+  <xr:revisionPtr revIDLastSave="286" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6F1B936-D5A0-447F-86D5-10FD26BBB65C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="📊 Project Overview" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="401">
   <si>
     <t>LINGUALLEARN AI - PROJECT TRACKER</t>
   </si>
@@ -1195,9 +1195,6 @@
     <t>AI Engineer Portfolio</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>Phase 3 - Multi-Modal Layer</t>
   </si>
   <si>
@@ -1249,13 +1246,13 @@
     <t>Reset Secret</t>
   </si>
   <si>
-    <t>58 / 120</t>
-  </si>
-  <si>
-    <t>51 (37%)</t>
-  </si>
-  <si>
-    <t>82 (60%)</t>
+    <t>62 / 120</t>
+  </si>
+  <si>
+    <t>61 (45%)</t>
+  </si>
+  <si>
+    <t>72 (53%)</t>
   </si>
 </sst>
 </file>
@@ -1335,7 +1332,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1402,6 +1399,12 @@
         <bgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1443,7 +1446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1514,7 +1517,6 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1524,6 +1526,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1727,8 +1733,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFC6EFCE"/>
       <color rgb="FFFFEB9C"/>
-      <color rgb="FFC6EFCE"/>
       <color rgb="FFFFC7CE"/>
     </mruColors>
   </colors>
@@ -2034,8 +2040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2050,100 +2056,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>380</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30" t="s">
-        <v>385</v>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
+      <c r="B5" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="30" t="s">
-        <v>382</v>
-      </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
+      <c r="B7" s="29" t="s">
+        <v>381</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="30" t="s">
-        <v>383</v>
-      </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
+      <c r="B8" s="29" t="s">
+        <v>382</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -2152,27 +2158,27 @@
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="30" t="s">
-        <v>384</v>
-      </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
+      <c r="B10" s="29" t="s">
+        <v>383</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
     </row>
     <row r="13" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
     </row>
     <row r="14" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -2263,8 +2269,8 @@
       <c r="B17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>381</v>
+      <c r="C17" s="34" t="s">
+        <v>20</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>30</v>
@@ -2274,7 +2280,7 @@
       </c>
       <c r="F17" s="16">
         <f>IFERROR(COUNTIF('Phase 3 - Multi-Modal'!E5:E105,"Complete")/COUNTA('Phase 3 - Multi-Modal'!A5:A105),0)</f>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="G17" s="4">
         <f>COUNTIF('Phase 3 - Multi-Modal'!E:E,"Blocked")</f>
@@ -2379,7 +2385,7 @@
         <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2403,7 +2409,7 @@
         <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -2422,7 +2428,7 @@
         <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -2465,24 +2471,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>331</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="4" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>332</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -2517,14 +2523,14 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="28" t="s">
         <v>341</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -2559,14 +2565,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="28" t="s">
         <v>350</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -2601,14 +2607,14 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="28" t="s">
         <v>359</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -2635,14 +2641,14 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="28" t="s">
         <v>366</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -2701,7 +2707,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
@@ -2712,18 +2718,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -3214,18 +3220,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -3897,15 +3903,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
@@ -3916,25 +3922,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>381</v>
+      <c r="B2" s="33" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -4151,7 +4157,7 @@
         <v>66</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>67</v>
@@ -4164,7 +4170,7 @@
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -4231,7 +4237,7 @@
         <v>83</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>66</v>
@@ -4259,7 +4265,7 @@
         <v>83</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>66</v>
@@ -4287,7 +4293,7 @@
         <v>83</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>66</v>
@@ -4315,7 +4321,7 @@
         <v>83</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>66</v>
@@ -4343,7 +4349,7 @@
         <v>83</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>66</v>
@@ -4389,10 +4395,10 @@
         <v>2.5</v>
       </c>
       <c r="I19" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="J19" s="10" t="s">
         <v>397</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -4437,7 +4443,7 @@
         <v>66</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>67</v>
@@ -4446,7 +4452,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
@@ -4465,7 +4471,7 @@
         <v>66</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>67</v>
@@ -4477,7 +4483,9 @@
         <v>0</v>
       </c>
       <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
+      <c r="J22" s="10" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
@@ -4493,7 +4501,7 @@
         <v>66</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>94</v>
@@ -4505,7 +4513,9 @@
         <v>0</v>
       </c>
       <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
+      <c r="J23" s="10" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
@@ -4521,7 +4531,7 @@
         <v>66</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>94</v>
@@ -4533,11 +4543,13 @@
         <v>0</v>
       </c>
       <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
+      <c r="J24" s="10" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>92</v>
@@ -4549,7 +4561,7 @@
         <v>66</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>94</v>
@@ -4558,14 +4570,14 @@
         <v>1</v>
       </c>
       <c r="H25" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>92</v>
@@ -4577,7 +4589,7 @@
         <v>66</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>94</v>
@@ -4586,14 +4598,14 @@
         <v>0.5</v>
       </c>
       <c r="H26" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>92</v>
@@ -4605,7 +4617,7 @@
         <v>66</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>67</v>
@@ -4621,7 +4633,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>92</v>
@@ -4633,7 +4645,7 @@
         <v>66</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>67</v>
@@ -4642,14 +4654,14 @@
         <v>1.5</v>
       </c>
       <c r="H28" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>92</v>
@@ -4661,7 +4673,7 @@
         <v>66</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>101</v>
@@ -4670,7 +4682,7 @@
         <v>0.5</v>
       </c>
       <c r="H29" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
@@ -4728,18 +4740,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -5394,18 +5406,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -6032,18 +6044,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -6697,17 +6709,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>311</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -6824,14 +6836,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>324</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">

</xml_diff>

<commit_message>
Built and trained ML Forgetting Curve model
</commit_message>
<xml_diff>
--- a/docs/Project_Tracker.xlsx
+++ b/docs/Project_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://potbelly-my.sharepoint.com/personal/anicia_clayton_potbelly_com/Documents/Desktop/linguallearn-portfolio/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="286" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6F1B936-D5A0-447F-86D5-10FD26BBB65C}"/>
+  <xr:revisionPtr revIDLastSave="330" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{217E4410-5670-495F-9628-C77FFC9E0A01}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="405">
   <si>
     <t>LINGUALLEARN AI - PROJECT TRACKER</t>
   </si>
@@ -1195,18 +1195,9 @@
     <t>AI Engineer Portfolio</t>
   </si>
   <si>
-    <t>Phase 3 - Multi-Modal Layer</t>
-  </si>
-  <si>
-    <t>Delayed a week</t>
-  </si>
-  <si>
     <t>AWS (VPC, EC2, RDS, Lambda, S3, CloudFront, ALB, CloudWatch, Secrets Manager), Terraform, Python, FastAPI, PostgreSQL</t>
   </si>
   <si>
-    <t>7 Weeks (90-120 hours total)</t>
-  </si>
-  <si>
     <t>Later enhancement</t>
   </si>
   <si>
@@ -1246,13 +1237,34 @@
     <t>Reset Secret</t>
   </si>
   <si>
-    <t>62 / 120</t>
-  </si>
-  <si>
-    <t>61 (45%)</t>
-  </si>
-  <si>
-    <t>72 (53%)</t>
+    <t>Future Demos</t>
+  </si>
+  <si>
+    <t>Furture Demos</t>
+  </si>
+  <si>
+    <t>Later Enhancement items</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>68.5 / 120</t>
+  </si>
+  <si>
+    <t>66 (48%)</t>
+  </si>
+  <si>
+    <t>67 (49%)</t>
+  </si>
+  <si>
+    <t>Phase 4 - ML Integration Layer</t>
+  </si>
+  <si>
+    <t>Delayed 2 weeks</t>
+  </si>
+  <si>
+    <t>8 Weeks (90-120 hours total)</t>
   </si>
 </sst>
 </file>
@@ -1446,7 +1458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1517,6 +1529,10 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1528,10 +1544,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1733,8 +1746,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFEB9C"/>
       <color rgb="FFC6EFCE"/>
-      <color rgb="FFFFEB9C"/>
       <color rgb="FFFFC7CE"/>
     </mruColors>
   </colors>
@@ -2040,8 +2053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2056,100 +2069,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="31" t="s">
         <v>380</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>384</v>
-      </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
+      <c r="B5" s="31" t="s">
+        <v>404</v>
+      </c>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="29" t="s">
-        <v>381</v>
-      </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
+      <c r="B7" s="31" t="s">
+        <v>402</v>
+      </c>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="29" t="s">
-        <v>382</v>
-      </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
+      <c r="B8" s="31" t="s">
+        <v>403</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -2158,27 +2171,27 @@
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>383</v>
-      </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
+      <c r="B10" s="31" t="s">
+        <v>381</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="13" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -2269,7 +2282,7 @@
       <c r="B17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="29" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -2286,7 +2299,9 @@
         <f>COUNTIF('Phase 3 - Multi-Modal'!E:E,"Blocked")</f>
         <v>0</v>
       </c>
-      <c r="H17" s="4"/>
+      <c r="H17" s="4" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
@@ -2295,8 +2310,8 @@
       <c r="B18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>29</v>
+      <c r="C18" s="15" t="s">
+        <v>398</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>33</v>
@@ -2306,7 +2321,7 @@
       </c>
       <c r="F18" s="16">
         <f>IFERROR(COUNTIF('Phase 4 - ML Integration'!E5:E100,"Complete")/COUNTA('Phase 4 - ML Integration'!A5:A100),0)</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G18" s="4">
         <f>COUNTIF('Phase 4 - ML Integration'!E:E,"Blocked")</f>
@@ -2385,7 +2400,7 @@
         <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2409,7 +2424,7 @@
         <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -2428,7 +2443,7 @@
         <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -2471,24 +2486,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>331</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="4" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="30" t="s">
         <v>332</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -2523,14 +2538,14 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="30" t="s">
         <v>341</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -2565,14 +2580,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="30" t="s">
         <v>350</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -2607,14 +2622,14 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="30" t="s">
         <v>359</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -2641,14 +2656,14 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="30" t="s">
         <v>366</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -2718,18 +2733,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -3220,18 +3235,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -3905,7 +3920,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3922,24 +3937,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="28" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4170,7 +4185,7 @@
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -4237,7 +4252,7 @@
         <v>83</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>66</v>
@@ -4265,7 +4280,7 @@
         <v>83</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>66</v>
@@ -4293,7 +4308,7 @@
         <v>83</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>66</v>
@@ -4321,7 +4336,7 @@
         <v>83</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>66</v>
@@ -4349,7 +4364,7 @@
         <v>83</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>66</v>
@@ -4395,10 +4410,10 @@
         <v>2.5</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -4484,7 +4499,7 @@
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="10" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -4514,7 +4529,7 @@
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="10" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -4544,12 +4559,12 @@
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>92</v>
@@ -4577,7 +4592,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>92</v>
@@ -4605,7 +4620,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>92</v>
@@ -4633,7 +4648,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>92</v>
@@ -4661,7 +4676,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>92</v>
@@ -4723,13 +4738,13 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:J1"/>
+      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
@@ -4740,25 +4755,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>29</v>
+      <c r="B2" s="35" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -4807,7 +4822,7 @@
         <v>66</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>67</v>
@@ -4816,7 +4831,7 @@
         <v>2</v>
       </c>
       <c r="H5" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
@@ -4835,7 +4850,7 @@
         <v>66</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>67</v>
@@ -4844,7 +4859,7 @@
         <v>1.5</v>
       </c>
       <c r="H6" s="10">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
@@ -4863,7 +4878,7 @@
         <v>66</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>67</v>
@@ -4872,7 +4887,7 @@
         <v>0.5</v>
       </c>
       <c r="H7" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
@@ -4891,7 +4906,7 @@
         <v>66</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>67</v>
@@ -4900,7 +4915,7 @@
         <v>0.5</v>
       </c>
       <c r="H8" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -5406,18 +5421,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -6044,18 +6059,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -6709,17 +6724,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -6836,14 +6851,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>324</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">

</xml_diff>

<commit_message>
Add ML inference Lambda with optimized layer (218MB unzipped)
</commit_message>
<xml_diff>
--- a/docs/Project_Tracker.xlsx
+++ b/docs/Project_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://potbelly-my.sharepoint.com/personal/anicia_clayton_potbelly_com/Documents/Desktop/linguallearn-portfolio/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="330" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{217E4410-5670-495F-9628-C77FFC9E0A01}"/>
+  <xr:revisionPtr revIDLastSave="376" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E33E9FA3-5744-4F97-A281-9E57EAB7E73C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="411">
   <si>
     <t>LINGUALLEARN AI - PROJECT TRACKER</t>
   </si>
@@ -1249,15 +1249,6 @@
     <t>In progress</t>
   </si>
   <si>
-    <t>68.5 / 120</t>
-  </si>
-  <si>
-    <t>66 (48%)</t>
-  </si>
-  <si>
-    <t>67 (49%)</t>
-  </si>
-  <si>
     <t>Phase 4 - ML Integration Layer</t>
   </si>
   <si>
@@ -1265,6 +1256,33 @@
   </si>
   <si>
     <t>8 Weeks (90-120 hours total)</t>
+  </si>
+  <si>
+    <t>Phase 3</t>
+  </si>
+  <si>
+    <t>API &amp; compute layer complete - 100%</t>
+  </si>
+  <si>
+    <t>Multi-Modal Activity Tracking complete - 97%</t>
+  </si>
+  <si>
+    <t>AWS Resource size limit</t>
+  </si>
+  <si>
+    <t>Lambda Layers to separate dependencies</t>
+  </si>
+  <si>
+    <t>70 (51%)</t>
+  </si>
+  <si>
+    <t>63 (46%)</t>
+  </si>
+  <si>
+    <t>76.5 / 120</t>
+  </si>
+  <si>
+    <t>Lambda size limit - optimization</t>
   </si>
 </sst>
 </file>
@@ -1458,7 +1476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1533,6 +1551,7 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1544,7 +1563,19 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2053,8 +2084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2069,100 +2100,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="32" t="s">
         <v>380</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="31" t="s">
-        <v>404</v>
-      </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
+      <c r="B5" s="32" t="s">
+        <v>401</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>402</v>
-      </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
+      <c r="B7" s="32" t="s">
+        <v>399</v>
+      </c>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>403</v>
-      </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
+      <c r="B8" s="32" t="s">
+        <v>400</v>
+      </c>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -2171,27 +2202,27 @@
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="32" t="s">
         <v>381</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
     </row>
     <row r="13" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -2321,13 +2352,15 @@
       </c>
       <c r="F18" s="16">
         <f>IFERROR(COUNTIF('Phase 4 - ML Integration'!E5:E100,"Complete")/COUNTA('Phase 4 - ML Integration'!A5:A100),0)</f>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="G18" s="4">
         <f>COUNTIF('Phase 4 - ML Integration'!E:E,"Blocked")</f>
         <v>0</v>
       </c>
-      <c r="H18" s="4"/>
+      <c r="H18" s="4" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
@@ -2400,7 +2433,7 @@
         <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2424,7 +2457,7 @@
         <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -2443,7 +2476,7 @@
         <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -2486,24 +2519,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>331</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="4" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="31" t="s">
         <v>332</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -2538,14 +2571,14 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -2580,14 +2613,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="31" t="s">
         <v>350</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -2622,14 +2655,14 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="31" t="s">
         <v>359</v>
       </c>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -2656,14 +2689,14 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="31" t="s">
         <v>366</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -2733,18 +2766,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -3235,18 +3268,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -3937,18 +3970,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4738,7 +4771,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4755,24 +4788,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="30" t="s">
         <v>398</v>
       </c>
     </row>
@@ -4934,7 +4967,7 @@
         <v>66</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>67</v>
@@ -4943,7 +4976,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -4962,7 +4995,7 @@
         <v>66</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>67</v>
@@ -4971,7 +5004,7 @@
         <v>1.5</v>
       </c>
       <c r="H10" s="10">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
@@ -4990,7 +5023,7 @@
         <v>66</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>67</v>
@@ -4999,7 +5032,7 @@
         <v>0.5</v>
       </c>
       <c r="H11" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -5018,7 +5051,7 @@
         <v>66</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>67</v>
@@ -5027,10 +5060,14 @@
         <v>1</v>
       </c>
       <c r="H12" s="10">
-        <v>0</v>
-      </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
@@ -5421,18 +5458,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -6059,18 +6096,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -6724,17 +6761,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>311</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -6834,10 +6871,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6851,14 +6888,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>324</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -6921,23 +6958,63 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="25">
+      <c r="A6" s="36">
         <v>45975</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="37" t="s">
         <v>317</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="37" t="s">
         <v>329</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="37" t="s">
         <v>379</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>67</v>
+      <c r="F6" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="38">
+        <v>45987</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>317</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>377</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>403</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="38">
+        <v>45998</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>402</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>377</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>404</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ML prediction API endpoints with database storage
</commit_message>
<xml_diff>
--- a/docs/Project_Tracker.xlsx
+++ b/docs/Project_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://potbelly-my.sharepoint.com/personal/anicia_clayton_potbelly_com/Documents/Desktop/linguallearn-portfolio/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="376" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E33E9FA3-5744-4F97-A281-9E57EAB7E73C}"/>
+  <xr:revisionPtr revIDLastSave="390" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA01F7CB-A576-49BC-89C3-6A10030AD7FD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="412">
   <si>
     <t>LINGUALLEARN AI - PROJECT TRACKER</t>
   </si>
@@ -1273,16 +1273,19 @@
     <t>Lambda Layers to separate dependencies</t>
   </si>
   <si>
-    <t>70 (51%)</t>
-  </si>
-  <si>
-    <t>63 (46%)</t>
-  </si>
-  <si>
-    <t>76.5 / 120</t>
-  </si>
-  <si>
     <t>Lambda size limit - optimization</t>
+  </si>
+  <si>
+    <t>Resolved a few errors</t>
+  </si>
+  <si>
+    <t>81.5 / 120</t>
+  </si>
+  <si>
+    <t>73 (53%)</t>
+  </si>
+  <si>
+    <t>60 (44%)</t>
   </si>
 </sst>
 </file>
@@ -1476,7 +1479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1552,6 +1555,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1563,19 +1576,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2084,8 +2084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2100,100 +2100,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="36" t="s">
         <v>380</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="36" t="s">
         <v>401</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="36" t="s">
         <v>399</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="36" t="s">
         <v>400</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -2202,27 +2202,27 @@
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="36" t="s">
         <v>381</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
     </row>
     <row r="13" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
     </row>
     <row r="14" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -2352,14 +2352,14 @@
       </c>
       <c r="F18" s="16">
         <f>IFERROR(COUNTIF('Phase 4 - ML Integration'!E5:E100,"Complete")/COUNTA('Phase 4 - ML Integration'!A5:A100),0)</f>
-        <v>0.4</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G18" s="4">
         <f>COUNTIF('Phase 4 - ML Integration'!E:E,"Blocked")</f>
         <v>0</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -2433,7 +2433,7 @@
         <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2457,7 +2457,7 @@
         <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -2519,24 +2519,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>331</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="4" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="35" t="s">
         <v>332</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -2571,14 +2571,14 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="35" t="s">
         <v>341</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -2613,14 +2613,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="35" t="s">
         <v>350</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -2655,14 +2655,14 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="35" t="s">
         <v>359</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -2689,14 +2689,14 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="35" t="s">
         <v>366</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -2766,18 +2766,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -3268,18 +3268,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -3970,18 +3970,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4771,7 +4771,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4788,18 +4788,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -5083,7 +5083,7 @@
         <v>66</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>67</v>
@@ -5092,7 +5092,7 @@
         <v>2</v>
       </c>
       <c r="H13" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
@@ -5111,7 +5111,7 @@
         <v>66</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>67</v>
@@ -5120,7 +5120,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
@@ -5139,7 +5139,7 @@
         <v>66</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>67</v>
@@ -5148,10 +5148,12 @@
         <v>1</v>
       </c>
       <c r="H15" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+      <c r="J15" s="10" t="s">
+        <v>408</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
@@ -5458,18 +5460,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -6096,18 +6098,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -6761,17 +6763,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="39" t="s">
         <v>311</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -6888,14 +6890,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>324</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -6958,62 +6960,62 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="36">
+      <c r="A6" s="31">
         <v>45975</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="37" t="s">
+      <c r="B6" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="32" t="s">
         <v>317</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="32" t="s">
         <v>329</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="32" t="s">
         <v>379</v>
       </c>
-      <c r="F6" s="37" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="40" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38">
+      <c r="F6" s="32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="33">
         <v>45987</v>
       </c>
-      <c r="B7" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="39" t="s">
+      <c r="B7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="F7" s="39" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="40" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38">
+      <c r="F7" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="33">
         <v>45998</v>
       </c>
-      <c r="B8" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="39" t="s">
+      <c r="B8" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>402</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="10" t="s">
         <v>404</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="10" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Week 4 documentation
</commit_message>
<xml_diff>
--- a/docs/Project_Tracker.xlsx
+++ b/docs/Project_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://potbelly-my.sharepoint.com/personal/anicia_clayton_potbelly_com/Documents/Desktop/linguallearn-portfolio/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="476" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E6742A7-11C2-4651-96B1-4F1B7579DEA0}"/>
+  <xr:revisionPtr revIDLastSave="492" documentId="8_{C9C18196-394D-4E08-AEE3-4532190AC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2B390FA-AB78-46FA-B695-B818AF2BA5DB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="420">
   <si>
     <t>LINGUALLEARN AI - PROJECT TRACKER</t>
   </si>
@@ -1181,9 +1181,6 @@
     <t>Git sync issue- nested repo + restructured folders</t>
   </si>
   <si>
-    <t>AI Engineer Portfolio</t>
-  </si>
-  <si>
     <t>AWS (VPC, EC2, RDS, Lambda, S3, CloudFront, ALB, CloudWatch, Secrets Manager), Terraform, Python, FastAPI, PostgreSQL</t>
   </si>
   <si>
@@ -1233,12 +1230,6 @@
   </si>
   <si>
     <t>Later Enhancement items</t>
-  </si>
-  <si>
-    <t>In progress</t>
-  </si>
-  <si>
-    <t>Phase 4 - ML Integration Layer</t>
   </si>
   <si>
     <t>Delayed 2 weeks</t>
@@ -1309,13 +1300,19 @@
 3. Dowload files</t>
   </si>
   <si>
-    <t>89.5 / 120</t>
-  </si>
-  <si>
-    <t>55 (40%)</t>
-  </si>
-  <si>
-    <t>78 (57%)</t>
+    <t>91.5 / 120</t>
+  </si>
+  <si>
+    <t>53 (40%)</t>
+  </si>
+  <si>
+    <t>80 (58%)</t>
+  </si>
+  <si>
+    <t>Phase 5 - Monitoring</t>
+  </si>
+  <si>
+    <t>MLOps Engineer Portfolio</t>
   </si>
 </sst>
 </file>
@@ -1526,7 +1523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1601,7 +1598,6 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1842,8 +1838,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFC6EFCE"/>
       <color rgb="FFFFEB9C"/>
-      <color rgb="FFC6EFCE"/>
       <color rgb="FFFFC7CE"/>
     </mruColors>
   </colors>
@@ -2149,8 +2145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2165,100 +2161,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="35" t="s">
-        <v>376</v>
-      </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
+      <c r="B4" s="34" t="s">
+        <v>419</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="35" t="s">
-        <v>397</v>
-      </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
+      <c r="B5" s="34" t="s">
+        <v>394</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>395</v>
-      </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
+      <c r="B7" s="34" t="s">
+        <v>418</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="35" t="s">
-        <v>396</v>
-      </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
+      <c r="B8" s="34" t="s">
+        <v>393</v>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -2267,27 +2263,27 @@
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="35" t="s">
-        <v>377</v>
-      </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
+      <c r="B10" s="34" t="s">
+        <v>376</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
     </row>
     <row r="13" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -2396,7 +2392,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -2406,8 +2402,8 @@
       <c r="B18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>394</v>
+      <c r="C18" s="29" t="s">
+        <v>20</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>32</v>
@@ -2417,14 +2413,14 @@
       </c>
       <c r="F18" s="16">
         <f>IFERROR(COUNTIF('Phase 4 - ML Integration'!E5:E100,"Complete")/COUNTA('Phase 4 - ML Integration'!A5:A100),0)</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G18" s="4">
         <f>COUNTIF('Phase 4 - ML Integration'!E:E,"Blocked")</f>
         <v>0</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -2498,7 +2494,7 @@
         <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2522,7 +2518,7 @@
         <v>47</v>
       </c>
       <c r="B28" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -2541,7 +2537,7 @@
         <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -2584,24 +2580,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>327</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="4" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>328</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -2636,14 +2632,14 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="33" t="s">
         <v>337</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -2678,14 +2674,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -2720,14 +2716,14 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="33" t="s">
         <v>355</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -2754,14 +2750,14 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="33" t="s">
         <v>362</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -2831,18 +2827,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -3333,18 +3329,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4035,18 +4031,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4283,7 +4279,7 @@
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -4350,7 +4346,7 @@
         <v>82</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>65</v>
@@ -4378,7 +4374,7 @@
         <v>82</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>65</v>
@@ -4406,7 +4402,7 @@
         <v>82</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>65</v>
@@ -4434,7 +4430,7 @@
         <v>82</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>65</v>
@@ -4462,7 +4458,7 @@
         <v>82</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>65</v>
@@ -4508,10 +4504,10 @@
         <v>2.5</v>
       </c>
       <c r="I19" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="J19" s="10" t="s">
         <v>389</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -4597,7 +4593,7 @@
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -4627,7 +4623,7 @@
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -4657,12 +4653,12 @@
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>91</v>
@@ -4690,7 +4686,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>91</v>
@@ -4718,7 +4714,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>91</v>
@@ -4746,7 +4742,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>91</v>
@@ -4774,7 +4770,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>91</v>
@@ -4836,7 +4832,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4853,25 +4849,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="30" t="s">
-        <v>394</v>
+      <c r="B2" s="28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -5128,10 +5124,10 @@
         <v>4</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -5217,7 +5213,7 @@
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -5246,10 +5242,10 @@
         <v>2</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -5260,7 +5256,7 @@
         <v>86</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>65</v>
@@ -5288,7 +5284,7 @@
         <v>86</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>65</v>
@@ -5316,7 +5312,7 @@
         <v>86</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>65</v>
@@ -5334,7 +5330,7 @@
         <v>2.5</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="J19" s="10"/>
     </row>
@@ -5365,7 +5361,7 @@
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="10" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -5395,7 +5391,7 @@
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="10" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -5440,7 +5436,7 @@
         <v>65</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>66</v>
@@ -5449,7 +5445,7 @@
         <v>1.5</v>
       </c>
       <c r="H23" s="10">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
@@ -5468,7 +5464,7 @@
         <v>65</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>100</v>
@@ -5477,7 +5473,7 @@
         <v>0.5</v>
       </c>
       <c r="H24" s="10">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
@@ -5509,6 +5505,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5535,18 +5532,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -6173,18 +6170,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>266</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -6838,17 +6835,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -6908,7 +6905,7 @@
         <v>45974</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="40" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="39" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>316</v>
       </c>
@@ -6938,31 +6935,31 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="41" t="s">
-        <v>416</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>407</v>
-      </c>
-      <c r="C6" s="41" t="s">
+      <c r="A6" s="40" t="s">
+        <v>413</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>404</v>
+      </c>
+      <c r="C6" s="40" t="s">
         <v>216</v>
       </c>
-      <c r="D6" s="41" t="s">
-        <v>415</v>
-      </c>
-      <c r="E6" s="44" t="s">
+      <c r="D6" s="40" t="s">
+        <v>412</v>
+      </c>
+      <c r="E6" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="40" t="s">
         <v>318</v>
       </c>
-      <c r="G6" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="43" t="s">
-        <v>417</v>
-      </c>
-      <c r="I6" s="42">
+      <c r="G6" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="42" t="s">
+        <v>414</v>
+      </c>
+      <c r="I6" s="41">
         <v>46017</v>
       </c>
     </row>
@@ -6994,14 +6991,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>320</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -7064,27 +7061,27 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="31">
+      <c r="A6" s="30">
         <v>45975</v>
       </c>
-      <c r="B6" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="32" t="s">
+      <c r="B6" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="31" t="s">
         <v>313</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="31" t="s">
         <v>325</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="31" t="s">
         <v>375</v>
       </c>
-      <c r="F6" s="32" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33">
+      <c r="F6" s="31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="32">
         <v>45987</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -7097,49 +7094,49 @@
         <v>373</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33">
+    <row r="8" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="32">
         <v>45998</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>65</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>373</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="33">
+    <row r="9" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="32">
         <v>46006</v>
       </c>
-      <c r="B9" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>407</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>408</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>409</v>
-      </c>
-      <c r="F9" s="39" t="s">
+      <c r="B9" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>404</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>405</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>406</v>
+      </c>
+      <c r="F9" s="38" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>